<commit_message>
Added conclusion, improved sequence prediction, added related work
</commit_message>
<xml_diff>
--- a/Thesis/files/Data All Users Combined.xlsx
+++ b/Thesis/files/Data All Users Combined.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17750" tabRatio="844" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17750" tabRatio="844" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="All Data" sheetId="2" r:id="rId1"/>
@@ -50233,7 +50233,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U30" sqref="U30"/>
     </sheetView>
   </sheetViews>
@@ -62224,8 +62224,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:J124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>